<commit_message>
se modifico el modal de solicitud de certificados y se corrigieron errores
</commit_message>
<xml_diff>
--- a/src/assets/archivos/PRIMARIA-INDIGENA.xlsx
+++ b/src/assets/archivos/PRIMARIA-INDIGENA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devel\Documents\desarrollo\HistoricoCalificaciones\HistoricosCalificaciones2\src\assets\archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5682567-6FE7-418A-A3E4-4E611F5C65F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF56D3C4-37CE-4D6C-A77D-346711E5D5EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C988C04A-2342-47BD-B2BC-ADB15F06BB9C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{C988C04A-2342-47BD-B2BC-ADB15F06BB9C}"/>
   </bookViews>
   <sheets>
     <sheet name="DE 1979-1991" sheetId="8" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="84">
   <si>
     <t>nombre</t>
   </si>
@@ -283,180 +283,6 @@
   </si>
   <si>
     <t>Lengua_indigena</t>
-  </si>
-  <si>
-    <t>alondra</t>
-  </si>
-  <si>
-    <t>gildardo</t>
-  </si>
-  <si>
-    <t>luis carlos</t>
-  </si>
-  <si>
-    <t>jose rodolfo</t>
-  </si>
-  <si>
-    <t>carlos</t>
-  </si>
-  <si>
-    <t>nilda leticia</t>
-  </si>
-  <si>
-    <t>benjamin</t>
-  </si>
-  <si>
-    <t>leocadio</t>
-  </si>
-  <si>
-    <t>rigoberto</t>
-  </si>
-  <si>
-    <t>cesar agripin</t>
-  </si>
-  <si>
-    <t>ana elda</t>
-  </si>
-  <si>
-    <t>olegario</t>
-  </si>
-  <si>
-    <t>aguilar</t>
-  </si>
-  <si>
-    <t>gutierres</t>
-  </si>
-  <si>
-    <t>carrillo</t>
-  </si>
-  <si>
-    <t>rodriguez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">de jesus </t>
-  </si>
-  <si>
-    <t>lopez</t>
-  </si>
-  <si>
-    <t>de la cruz</t>
-  </si>
-  <si>
-    <t>lamas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">flores </t>
-  </si>
-  <si>
-    <t>de jesus</t>
-  </si>
-  <si>
-    <t>flores</t>
-  </si>
-  <si>
-    <t>lino</t>
-  </si>
-  <si>
-    <t>madera</t>
-  </si>
-  <si>
-    <t>zeferino</t>
-  </si>
-  <si>
-    <t>garcia</t>
-  </si>
-  <si>
-    <t>vargas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gonzales </t>
-  </si>
-  <si>
-    <t>T1325476</t>
-  </si>
-  <si>
-    <t>T1325477</t>
-  </si>
-  <si>
-    <t>T1325478</t>
-  </si>
-  <si>
-    <t>T1325479</t>
-  </si>
-  <si>
-    <t>T1325480</t>
-  </si>
-  <si>
-    <t>T1325481</t>
-  </si>
-  <si>
-    <t>T1325482</t>
-  </si>
-  <si>
-    <t>T1325483</t>
-  </si>
-  <si>
-    <t>T1325484</t>
-  </si>
-  <si>
-    <t>T1325485</t>
-  </si>
-  <si>
-    <t>T1325486</t>
-  </si>
-  <si>
-    <t>T1325487</t>
-  </si>
-  <si>
-    <t>18drp0006z</t>
-  </si>
-  <si>
-    <t>pentecatl (el sacerdote del vino)</t>
-  </si>
-  <si>
-    <t>ruiz</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>AUGA960508MNTGTL06</t>
-  </si>
-  <si>
-    <t>CARG960522HNTRDL07</t>
-  </si>
-  <si>
-    <t>JELL951223HNTSPS04</t>
-  </si>
-  <si>
-    <t>JEZR960630HNTSFDO7</t>
-  </si>
-  <si>
-    <t>CULC960414HNTRMR08</t>
-  </si>
-  <si>
-    <t>FOJN960229MNTLSL08</t>
-  </si>
-  <si>
-    <t>FOCB950331HNTLRN02</t>
-  </si>
-  <si>
-    <t>FOFL960213HNTLLC05</t>
-  </si>
-  <si>
-    <t>FOLR960104HNTLNG06</t>
-  </si>
-  <si>
-    <t>FOMC951216HNTLDS03</t>
-  </si>
-  <si>
-    <t>GAVA960125MNTRRN02</t>
-  </si>
-  <si>
-    <t>GOLO940909HNTNML05</t>
-  </si>
-  <si>
-    <t>B</t>
   </si>
   <si>
     <t>PLAN 1975 POR AREAS O ASIG INDIGENA.</t>
@@ -2732,8 +2558,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:X99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2834,903 +2660,351 @@
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="K2" s="7">
-        <v>101</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="P2" s="16">
-        <v>7.8</v>
-      </c>
-      <c r="Q2" s="16">
-        <v>8.4</v>
-      </c>
-      <c r="R2" s="16">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="S2" s="16">
-        <v>8</v>
-      </c>
-      <c r="T2" s="16">
-        <v>8.4</v>
-      </c>
-      <c r="U2" s="16">
-        <v>8</v>
-      </c>
-      <c r="V2" s="16">
-        <v>8.4</v>
-      </c>
-      <c r="W2" s="16">
-        <v>8</v>
-      </c>
-      <c r="X2" s="19">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="19" t="e">
         <f>AVERAGE(Tabla3235672[[#This Row],[Lengua_indigena]:[Educacion_tecnologica]])</f>
-        <v>8.1499999999999986</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="K3" s="7">
-        <v>101</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O3" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="P3" s="16">
-        <v>7.4</v>
-      </c>
-      <c r="Q3" s="16">
-        <v>7.8</v>
-      </c>
-      <c r="R3" s="16">
-        <v>7.4</v>
-      </c>
-      <c r="S3" s="16">
-        <v>8</v>
-      </c>
-      <c r="T3" s="16">
-        <v>7</v>
-      </c>
-      <c r="U3" s="16">
-        <v>7.8</v>
-      </c>
-      <c r="V3" s="16">
-        <v>7.4</v>
-      </c>
-      <c r="W3" s="16">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="X3" s="19">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="16"/>
+      <c r="U3" s="16"/>
+      <c r="V3" s="16"/>
+      <c r="W3" s="16"/>
+      <c r="X3" s="19" t="e">
         <f>AVERAGE(Tabla3235672[[#This Row],[Lengua_indigena]:[Educacion_tecnologica]])</f>
-        <v>7.625</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="K4" s="7">
-        <v>101</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O4" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="P4" s="16">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="Q4" s="16">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="R4" s="16">
-        <v>8.4</v>
-      </c>
-      <c r="S4" s="16">
-        <v>8</v>
-      </c>
-      <c r="T4" s="16">
-        <v>7.8</v>
-      </c>
-      <c r="U4" s="16">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="V4" s="16">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="W4" s="16">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="X4" s="19">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="19" t="e">
         <f>AVERAGE(Tabla3235672[[#This Row],[Lengua_indigena]:[Educacion_tecnologica]])</f>
-        <v>8.3749999999999982</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="K5" s="7">
-        <v>101</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O5" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="P5" s="16">
-        <v>7.6</v>
-      </c>
-      <c r="Q5" s="16">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="R5" s="16">
-        <v>8.4</v>
-      </c>
-      <c r="S5" s="16">
-        <v>8</v>
-      </c>
-      <c r="T5" s="16">
-        <v>8.6</v>
-      </c>
-      <c r="U5" s="16">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="V5" s="16">
-        <v>8.6</v>
-      </c>
-      <c r="W5" s="16">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="X5" s="19">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="16"/>
+      <c r="W5" s="16"/>
+      <c r="X5" s="19" t="e">
         <f>AVERAGE(Tabla3235672[[#This Row],[Lengua_indigena]:[Educacion_tecnologica]])</f>
-        <v>8.2999999999999989</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="K6" s="7">
-        <v>101</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O6" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="P6" s="16">
-        <v>7.4</v>
-      </c>
-      <c r="Q6" s="16">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="R6" s="16">
-        <v>8.5</v>
-      </c>
-      <c r="S6" s="16">
-        <v>8</v>
-      </c>
-      <c r="T6" s="16">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="U6" s="16">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="V6" s="16">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="W6" s="16">
-        <v>8.6</v>
-      </c>
-      <c r="X6" s="19">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="19" t="e">
         <f>AVERAGE(Tabla3235672[[#This Row],[Lengua_indigena]:[Educacion_tecnologica]])</f>
-        <v>8.3249999999999993</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="K7" s="7">
-        <v>101</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="N7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O7" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="P7" s="16">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="Q7" s="16">
-        <v>8.86</v>
-      </c>
-      <c r="R7" s="16">
-        <v>8.66</v>
-      </c>
-      <c r="S7" s="16">
-        <v>8</v>
-      </c>
-      <c r="T7" s="16">
-        <v>8.44</v>
-      </c>
-      <c r="U7" s="16">
-        <v>8.4</v>
-      </c>
-      <c r="V7" s="16">
-        <v>9</v>
-      </c>
-      <c r="W7" s="16">
-        <v>8.7200000000000006</v>
-      </c>
-      <c r="X7" s="19">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="16"/>
+      <c r="W7" s="16"/>
+      <c r="X7" s="19" t="e">
         <f>AVERAGE(Tabla3235672[[#This Row],[Lengua_indigena]:[Educacion_tecnologica]])</f>
-        <v>8.66</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="K8" s="7">
-        <v>101</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="M8" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="N8" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O8" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="P8" s="16">
-        <v>8</v>
-      </c>
-      <c r="Q8" s="16">
-        <v>9.02</v>
-      </c>
-      <c r="R8" s="16">
-        <v>8.82</v>
-      </c>
-      <c r="S8" s="16">
-        <v>8</v>
-      </c>
-      <c r="T8" s="16">
-        <v>8.58</v>
-      </c>
-      <c r="U8" s="16">
-        <v>8.5</v>
-      </c>
-      <c r="V8" s="16">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="W8" s="16">
-        <v>8.84</v>
-      </c>
-      <c r="X8" s="19">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="16"/>
+      <c r="V8" s="16"/>
+      <c r="W8" s="16"/>
+      <c r="X8" s="19" t="e">
         <f>AVERAGE(Tabla3235672[[#This Row],[Lengua_indigena]:[Educacion_tecnologica]])</f>
-        <v>8.620000000000001</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="K9" s="7">
-        <v>101</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O9" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="P9" s="16">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="Q9" s="16">
-        <v>9.18</v>
-      </c>
-      <c r="R9" s="16">
-        <v>8.98</v>
-      </c>
-      <c r="S9" s="16">
-        <v>8</v>
-      </c>
-      <c r="T9" s="16">
-        <v>8.7200000000000006</v>
-      </c>
-      <c r="U9" s="16">
-        <v>8.6</v>
-      </c>
-      <c r="V9" s="16">
-        <v>9.4</v>
-      </c>
-      <c r="W9" s="16">
-        <v>8.9600000000000009</v>
-      </c>
-      <c r="X9" s="19">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="16"/>
+      <c r="V9" s="16"/>
+      <c r="W9" s="16"/>
+      <c r="X9" s="19" t="e">
         <f>AVERAGE(Tabla3235672[[#This Row],[Lengua_indigena]:[Educacion_tecnologica]])</f>
-        <v>8.83</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="K10" s="7">
-        <v>101</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="M10" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="N10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O10" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="P10" s="16">
-        <v>9.1</v>
-      </c>
-      <c r="Q10" s="16">
-        <v>9.34</v>
-      </c>
-      <c r="R10" s="16">
-        <v>9.14</v>
-      </c>
-      <c r="S10" s="16">
-        <v>8</v>
-      </c>
-      <c r="T10" s="16">
-        <v>8.86</v>
-      </c>
-      <c r="U10" s="16">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="V10" s="16">
-        <v>9.6</v>
-      </c>
-      <c r="W10" s="16">
-        <v>9.08</v>
-      </c>
-      <c r="X10" s="19">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="16"/>
+      <c r="V10" s="16"/>
+      <c r="W10" s="16"/>
+      <c r="X10" s="19" t="e">
         <f>AVERAGE(Tabla3235672[[#This Row],[Lengua_indigena]:[Educacion_tecnologica]])</f>
-        <v>8.9775000000000009</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="K11" s="7">
-        <v>101</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="M11" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="N11" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O11" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="P11" s="16">
-        <v>9.4</v>
-      </c>
-      <c r="Q11" s="16">
-        <v>9.5</v>
-      </c>
-      <c r="R11" s="16">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="S11" s="16">
-        <v>8</v>
-      </c>
-      <c r="T11" s="16">
-        <v>9</v>
-      </c>
-      <c r="U11" s="16">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="V11" s="16">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="W11" s="16">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="X11" s="19">
+      <c r="A11" s="6"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="16"/>
+      <c r="V11" s="16"/>
+      <c r="W11" s="16"/>
+      <c r="X11" s="19" t="e">
         <f>AVERAGE(Tabla3235672[[#This Row],[Lengua_indigena]:[Educacion_tecnologica]])</f>
-        <v>9.125</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="K12" s="7">
-        <v>101</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="M12" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="N12" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O12" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="P12" s="16">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="Q12" s="16">
-        <v>9.66</v>
-      </c>
-      <c r="R12" s="16">
-        <v>9.4600000000000009</v>
-      </c>
-      <c r="S12" s="16">
-        <v>8</v>
-      </c>
-      <c r="T12" s="16">
-        <v>9.14</v>
-      </c>
-      <c r="U12" s="16">
-        <v>8.9</v>
-      </c>
-      <c r="V12" s="16">
-        <v>10</v>
-      </c>
-      <c r="W12" s="16">
-        <v>9.32</v>
-      </c>
-      <c r="X12" s="19">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="16"/>
+      <c r="V12" s="16"/>
+      <c r="W12" s="16"/>
+      <c r="X12" s="19" t="e">
         <f>AVERAGE(Tabla3235672[[#This Row],[Lengua_indigena]:[Educacion_tecnologica]])</f>
-        <v>9.2725000000000009</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="K13" s="7">
-        <v>101</v>
-      </c>
-      <c r="L13" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="M13" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="N13" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O13" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="P13" s="16">
-        <v>10</v>
-      </c>
-      <c r="Q13" s="16">
-        <v>9.82</v>
-      </c>
-      <c r="R13" s="16">
-        <v>9.4600000000000009</v>
-      </c>
-      <c r="S13" s="16">
-        <v>8</v>
-      </c>
-      <c r="T13" s="16">
-        <v>9.2799999999999994</v>
-      </c>
-      <c r="U13" s="16">
-        <v>9</v>
-      </c>
-      <c r="V13" s="16">
-        <v>5</v>
-      </c>
-      <c r="W13" s="16">
-        <v>9.44</v>
-      </c>
-      <c r="X13" s="19">
+      <c r="A13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="16"/>
+      <c r="T13" s="16"/>
+      <c r="U13" s="16"/>
+      <c r="V13" s="16"/>
+      <c r="W13" s="16"/>
+      <c r="X13" s="19" t="e">
         <f>AVERAGE(Tabla3235672[[#This Row],[Lengua_indigena]:[Educacion_tecnologica]])</f>
-        <v>8.75</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.3">
@@ -6031,8 +5305,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:Y99"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y14" sqref="Y14:Y99"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X2" sqref="A2:X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6137,939 +5411,363 @@
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="K2" s="7">
-        <v>101</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="P2" s="16">
-        <v>7.8</v>
-      </c>
-      <c r="Q2" s="16">
-        <v>10</v>
-      </c>
-      <c r="R2" s="16">
-        <v>7.8</v>
-      </c>
-      <c r="S2" s="16">
-        <v>8.4</v>
-      </c>
-      <c r="T2" s="16">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="U2" s="16">
-        <v>8</v>
-      </c>
-      <c r="V2" s="16">
-        <v>8.4</v>
-      </c>
-      <c r="W2" s="16">
-        <v>8</v>
-      </c>
-      <c r="X2" s="16">
-        <v>8.4</v>
-      </c>
-      <c r="Y2" s="16">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="16"/>
+      <c r="Y2" s="16" t="e">
         <f>AVERAGE(Tabla32356[[#This Row],[Lengua_indigena]:[Educacion_fisica]])</f>
-        <v>8.3333333333333339</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="K3" s="7">
-        <v>101</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O3" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="P3" s="16">
-        <v>7.4</v>
-      </c>
-      <c r="Q3" s="16">
-        <v>10</v>
-      </c>
-      <c r="R3" s="16">
-        <v>7.4</v>
-      </c>
-      <c r="S3" s="16">
-        <v>7.8</v>
-      </c>
-      <c r="T3" s="16">
-        <v>7.4</v>
-      </c>
-      <c r="U3" s="16">
-        <v>8</v>
-      </c>
-      <c r="V3" s="16">
-        <v>7</v>
-      </c>
-      <c r="W3" s="16">
-        <v>7.8</v>
-      </c>
-      <c r="X3" s="16">
-        <v>7.4</v>
-      </c>
-      <c r="Y3" s="16">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="16"/>
+      <c r="U3" s="16"/>
+      <c r="V3" s="16"/>
+      <c r="W3" s="16"/>
+      <c r="X3" s="16"/>
+      <c r="Y3" s="16" t="e">
         <f>AVERAGE(Tabla32356[[#This Row],[Lengua_indigena]:[Educacion_fisica]])</f>
-        <v>7.7999999999999989</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="K4" s="7">
-        <v>101</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O4" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="P4" s="16">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="Q4" s="16">
-        <v>10</v>
-      </c>
-      <c r="R4" s="16">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="S4" s="16">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="T4" s="16">
-        <v>8.4</v>
-      </c>
-      <c r="U4" s="16">
-        <v>8</v>
-      </c>
-      <c r="V4" s="16">
-        <v>7.8</v>
-      </c>
-      <c r="W4" s="16">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="X4" s="16">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="Y4" s="16">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16" t="e">
         <f>AVERAGE(Tabla32356[[#This Row],[Lengua_indigena]:[Educacion_fisica]])</f>
-        <v>8.5555555555555536</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="K5" s="7">
-        <v>101</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O5" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="P5" s="16">
-        <v>7.6</v>
-      </c>
-      <c r="Q5" s="16">
-        <v>10</v>
-      </c>
-      <c r="R5" s="16">
-        <v>7.6</v>
-      </c>
-      <c r="S5" s="16">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="T5" s="16">
-        <v>8.4</v>
-      </c>
-      <c r="U5" s="16">
-        <v>8</v>
-      </c>
-      <c r="V5" s="16">
-        <v>8.6</v>
-      </c>
-      <c r="W5" s="16">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="X5" s="16">
-        <v>8.6</v>
-      </c>
-      <c r="Y5" s="16">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="16"/>
+      <c r="W5" s="16"/>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="16" t="e">
         <f>AVERAGE(Tabla32356[[#This Row],[Lengua_indigena]:[Educacion_fisica]])</f>
-        <v>8.4222222222222225</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="K6" s="7">
-        <v>101</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O6" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="P6" s="16">
-        <v>7.4</v>
-      </c>
-      <c r="Q6" s="16">
-        <v>10</v>
-      </c>
-      <c r="R6" s="16">
-        <v>7.4</v>
-      </c>
-      <c r="S6" s="16">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="T6" s="16">
-        <v>8.5</v>
-      </c>
-      <c r="U6" s="16">
-        <v>8</v>
-      </c>
-      <c r="V6" s="16">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="W6" s="16">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="X6" s="16">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="Y6" s="16">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="16" t="e">
         <f>AVERAGE(Tabla32356[[#This Row],[Lengua_indigena]:[Educacion_fisica]])</f>
-        <v>8.3777777777777764</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="K7" s="7">
-        <v>101</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="N7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O7" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="P7" s="16">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="Q7" s="16">
-        <v>10</v>
-      </c>
-      <c r="R7" s="16">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="S7" s="16">
-        <v>8.86</v>
-      </c>
-      <c r="T7" s="16">
-        <v>8.66</v>
-      </c>
-      <c r="U7" s="16">
-        <v>8</v>
-      </c>
-      <c r="V7" s="16">
-        <v>8.44</v>
-      </c>
-      <c r="W7" s="16">
-        <v>8.4</v>
-      </c>
-      <c r="X7" s="16">
-        <v>9</v>
-      </c>
-      <c r="Y7" s="16">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="16"/>
+      <c r="W7" s="16"/>
+      <c r="X7" s="16"/>
+      <c r="Y7" s="16" t="e">
         <f>AVERAGE(Tabla32356[[#This Row],[Lengua_indigena]:[Educacion_fisica]])</f>
-        <v>8.862222222222222</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="K8" s="7">
-        <v>101</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="M8" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="N8" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O8" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="P8" s="16">
-        <v>8</v>
-      </c>
-      <c r="Q8" s="16">
-        <v>10</v>
-      </c>
-      <c r="R8" s="16">
-        <v>8</v>
-      </c>
-      <c r="S8" s="16">
-        <v>9.02</v>
-      </c>
-      <c r="T8" s="16">
-        <v>8.82</v>
-      </c>
-      <c r="U8" s="16">
-        <v>8</v>
-      </c>
-      <c r="V8" s="16">
-        <v>8.58</v>
-      </c>
-      <c r="W8" s="16">
-        <v>8.5</v>
-      </c>
-      <c r="X8" s="16">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="Y8" s="16">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="16"/>
+      <c r="V8" s="16"/>
+      <c r="W8" s="16"/>
+      <c r="X8" s="16"/>
+      <c r="Y8" s="16" t="e">
         <f>AVERAGE(Tabla32356[[#This Row],[Lengua_indigena]:[Educacion_fisica]])</f>
-        <v>8.68</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="K9" s="7">
-        <v>101</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O9" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="P9" s="16">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="Q9" s="16">
-        <v>10</v>
-      </c>
-      <c r="R9" s="16">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="S9" s="16">
-        <v>9.18</v>
-      </c>
-      <c r="T9" s="16">
-        <v>8.98</v>
-      </c>
-      <c r="U9" s="16">
-        <v>8</v>
-      </c>
-      <c r="V9" s="16">
-        <v>8.7200000000000006</v>
-      </c>
-      <c r="W9" s="16">
-        <v>8.6</v>
-      </c>
-      <c r="X9" s="16">
-        <v>9.4</v>
-      </c>
-      <c r="Y9" s="16">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="16"/>
+      <c r="V9" s="16"/>
+      <c r="W9" s="16"/>
+      <c r="X9" s="16"/>
+      <c r="Y9" s="16" t="e">
         <f>AVERAGE(Tabla32356[[#This Row],[Lengua_indigena]:[Educacion_fisica]])</f>
-        <v>8.9422222222222221</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="K10" s="7">
-        <v>101</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="M10" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="N10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O10" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="P10" s="16">
-        <v>9.1</v>
-      </c>
-      <c r="Q10" s="16">
-        <v>10</v>
-      </c>
-      <c r="R10" s="16">
-        <v>9.1</v>
-      </c>
-      <c r="S10" s="16">
-        <v>9.34</v>
-      </c>
-      <c r="T10" s="16">
-        <v>9.14</v>
-      </c>
-      <c r="U10" s="16">
-        <v>8</v>
-      </c>
-      <c r="V10" s="16">
-        <v>8.86</v>
-      </c>
-      <c r="W10" s="16">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="X10" s="16">
-        <v>9.6</v>
-      </c>
-      <c r="Y10" s="16">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="16"/>
+      <c r="V10" s="16"/>
+      <c r="W10" s="16"/>
+      <c r="X10" s="16"/>
+      <c r="Y10" s="16" t="e">
         <f>AVERAGE(Tabla32356[[#This Row],[Lengua_indigena]:[Educacion_fisica]])</f>
-        <v>9.0933333333333337</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="K11" s="7">
-        <v>101</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="M11" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="N11" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O11" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="P11" s="16">
-        <v>9.4</v>
-      </c>
-      <c r="Q11" s="16">
-        <v>10</v>
-      </c>
-      <c r="R11" s="16">
-        <v>9.4</v>
-      </c>
-      <c r="S11" s="16">
-        <v>9.5</v>
-      </c>
-      <c r="T11" s="16">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="U11" s="16">
-        <v>8</v>
-      </c>
-      <c r="V11" s="16">
-        <v>9</v>
-      </c>
-      <c r="W11" s="16">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="X11" s="16">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="Y11" s="16">
+      <c r="A11" s="6"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="16"/>
+      <c r="V11" s="16"/>
+      <c r="W11" s="16"/>
+      <c r="X11" s="16"/>
+      <c r="Y11" s="16" t="e">
         <f>AVERAGE(Tabla32356[[#This Row],[Lengua_indigena]:[Educacion_fisica]])</f>
-        <v>9.2444444444444436</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="K12" s="7">
-        <v>101</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="M12" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="N12" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O12" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="P12" s="16">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="Q12" s="16">
-        <v>10</v>
-      </c>
-      <c r="R12" s="16">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="S12" s="16">
-        <v>9.66</v>
-      </c>
-      <c r="T12" s="16">
-        <v>9.4600000000000009</v>
-      </c>
-      <c r="U12" s="16">
-        <v>8</v>
-      </c>
-      <c r="V12" s="16">
-        <v>9.14</v>
-      </c>
-      <c r="W12" s="16">
-        <v>8.9</v>
-      </c>
-      <c r="X12" s="16">
-        <v>10</v>
-      </c>
-      <c r="Y12" s="16">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="16"/>
+      <c r="V12" s="16"/>
+      <c r="W12" s="16"/>
+      <c r="X12" s="16"/>
+      <c r="Y12" s="16" t="e">
         <f>AVERAGE(Tabla32356[[#This Row],[Lengua_indigena]:[Educacion_fisica]])</f>
-        <v>9.3955555555555552</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="K13" s="7">
-        <v>101</v>
-      </c>
-      <c r="L13" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="M13" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="N13" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O13" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="P13" s="16">
-        <v>10</v>
-      </c>
-      <c r="Q13" s="16">
-        <v>10</v>
-      </c>
-      <c r="R13" s="16">
-        <v>10</v>
-      </c>
-      <c r="S13" s="16">
-        <v>9.82</v>
-      </c>
-      <c r="T13" s="16">
-        <v>9.4600000000000009</v>
-      </c>
-      <c r="U13" s="16">
-        <v>8</v>
-      </c>
-      <c r="V13" s="16">
-        <v>9.2799999999999994</v>
-      </c>
-      <c r="W13" s="16">
-        <v>9</v>
-      </c>
-      <c r="X13" s="16">
-        <v>5</v>
-      </c>
-      <c r="Y13" s="16">
+      <c r="A13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="16"/>
+      <c r="T13" s="16"/>
+      <c r="U13" s="16"/>
+      <c r="V13" s="16"/>
+      <c r="W13" s="16"/>
+      <c r="X13" s="16"/>
+      <c r="Y13" s="16" t="e">
         <f>AVERAGE(Tabla32356[[#This Row],[Lengua_indigena]:[Educacion_fisica]])</f>
-        <v>8.9511111111111106</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
@@ -9469,7 +8167,7 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:V99"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
@@ -12030,7 +10728,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>140</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
@@ -12046,7 +10744,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>141</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>

</xml_diff>